<commit_message>
Feature: Docs of Flask app with dynamic key functionalty of video encyrption - F_2 commit
</commit_message>
<xml_diff>
--- a/docs/results comparision Book1.xlsx
+++ b/docs/results comparision Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malateef\Desktop\FlaskVideoStreamingApp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93CC7A0-9F5A-4287-A1AA-3EBED2FDA18A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C71007-29CD-4BB9-A4CD-FB0512088D93}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{622DA7F2-D2C2-454C-A8C1-943429CB04DF}"/>
   </bookViews>
@@ -57,17 +57,17 @@
     <t>NHMK algorithm stats for 15.4 mb video</t>
   </si>
   <si>
-    <t>Novel Hybrid MultiKey algorithm</t>
+    <t>Hybrid Dynamic Key Video Encryption Algorithm (HDKVEA)</t>
   </si>
   <si>
-    <t>CipherShield algorithm</t>
+    <t>Novel Hybrid Multi Key Algorithm(NHMKA)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,6 +80,20 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -117,7 +131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -128,15 +142,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -188,7 +206,11 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-IN"/>
+              <a:rPr lang="en-IN">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Results comparision for 15.4mb video file</a:t>
             </a:r>
           </a:p>
@@ -239,7 +261,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Novel Hybrid MultiKey algorithm</c:v>
+                  <c:v>Novel Hybrid Multi Key Algorithm(NHMKA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -291,6 +313,28 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.908936226499041E-2"/>
+                  <c:y val="-3.4116285610015208E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-5151-4920-8C9F-AA2FC2E5199D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:solidFill>
                 <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -314,10 +358,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -406,14 +447,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CipherShield algorithm</c:v>
+                  <c:v>Hybrid Dynamic Key Video Encryption Algorithm (HDKVEA)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B0F0"/>
+              <a:srgbClr val="FFFF00"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -422,6 +463,94 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0"/>
+                  <c:y val="-2.779329117685397E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000004-5151-4920-8C9F-AA2FC2E5199D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="1"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="2.1816414017131948E-2"/>
+                  <c:y val="-4.2977836255643914E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-5151-4920-8C9F-AA2FC2E5199D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-8.1811552564245611E-3"/>
+                  <c:y val="-3.5012021933762301E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-5151-4920-8C9F-AA2FC2E5199D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="1.3635258760706435E-3"/>
+                  <c:y val="-3.587083380351002E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="outEnd"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="1"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-5151-4920-8C9F-AA2FC2E5199D}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:solidFill>
                 <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -445,10 +574,7 @@
                 <a:pPr>
                   <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="dk1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -568,14 +694,26 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IN"/>
+                  <a:rPr lang="en-IN">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Attributes</a:t>
                 </a:r>
                 <a:r>
-                  <a:rPr lang="en-IN" baseline="0"/>
-                  <a:t> for comparision</a:t>
+                  <a:rPr lang="en-IN" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> for Comparision</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-IN"/>
+                <a:endParaRPr lang="en-IN">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
               </a:p>
             </c:rich>
           </c:tx>
@@ -626,10 +764,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -676,10 +811,7 @@
                 <a:pPr>
                   <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
+                      <a:schemeClr val="tx1"/>
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
@@ -687,7 +819,11 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IN"/>
+                  <a:rPr lang="en-IN">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
                   <a:t>Time in Sec</a:t>
                 </a:r>
               </a:p>
@@ -708,10 +844,7 @@
               <a:pPr>
                 <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
+                    <a:schemeClr val="tx1"/>
                   </a:solidFill>
                   <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
@@ -740,10 +873,7 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
@@ -782,10 +912,7 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
+                <a:schemeClr val="tx1"/>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
@@ -1711,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{293C4CBE-BE60-4178-A265-B28159F92E2E}">
   <dimension ref="A4:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S32" sqref="S32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1723,15 +1850,15 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:5" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -1784,49 +1911,49 @@
       <c r="D9" s="2"/>
     </row>
     <row r="12" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="A16" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>